<commit_message>
pds 0.53 - pages11, 12, 21 and 22
</commit_message>
<xml_diff>
--- a/pkg/generators/pds/2022-11-28_ZEW_Survey.xlsx
+++ b/pkg/generators/pds/2022-11-28_ZEW_Survey.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3816" yWindow="3816" windowWidth="21600" windowHeight="11388" activeTab="2"/>
+    <workbookView xWindow="3816" yWindow="3816" windowWidth="21600" windowHeight="11388"/>
   </bookViews>
   <sheets>
     <sheet name="Direct Lending" sheetId="4" r:id="rId1"/>
@@ -929,13 +929,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1140,80 +1147,81 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1496,17 +1504,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W104"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="52.88671875" style="41" customWidth="1"/>
-    <col min="2" max="2" width="48.109375" style="48" customWidth="1"/>
+    <col min="2" max="2" width="45.77734375" style="48" customWidth="1"/>
     <col min="3" max="5" width="24.109375" style="41" customWidth="1"/>
     <col min="6" max="6" width="113.5546875" style="41" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="24.109375" style="41" customWidth="1"/>
@@ -2728,7 +2736,7 @@
       <c r="E50" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F50" s="18" t="s">
+      <c r="F50" s="51" t="s">
         <v>172</v>
       </c>
       <c r="G50" s="18" t="s">
@@ -2754,7 +2762,7 @@
       <c r="E51" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F51" s="18" t="s">
+      <c r="F51" s="51" t="s">
         <v>173</v>
       </c>
       <c r="G51" s="18" t="s">
@@ -3804,7 +3812,7 @@
       <c r="H99" s="40"/>
       <c r="I99" s="40"/>
     </row>
-    <row r="100" spans="1:23" s="39" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" s="39" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B100" s="6" t="s">
         <v>67</v>
       </c>
@@ -3913,11 +3921,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V104"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4347,9 +4355,9 @@
       </c>
       <c r="V19" s="39"/>
     </row>
-    <row r="20" spans="1:22" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39" t="s">
-        <v>126</v>
+    <row r="20" spans="1:22" s="44" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="50" t="s">
+        <v>271</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>125</v>
@@ -5973,7 +5981,7 @@
       <c r="G99" s="40"/>
       <c r="H99" s="40"/>
     </row>
-    <row r="100" spans="1:22" s="39" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:22" s="39" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B100" s="6" t="s">
         <v>67</v>
       </c>
@@ -6080,11 +6088,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomRight" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6405,7 +6413,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="44" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" s="44" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="50" t="s">
         <v>270</v>
       </c>

</xml_diff>

<commit_message>
pds 0.56 - ac2, ac3 specific questions
</commit_message>
<xml_diff>
--- a/pkg/generators/pds/2022-11-28_ZEW_Survey.xlsx
+++ b/pkg/generators/pds/2022-11-28_ZEW_Survey.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3816" yWindow="3816" windowWidth="21600" windowHeight="11388"/>
+    <workbookView xWindow="3816" yWindow="3816" windowWidth="21600" windowHeight="11388" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Direct Lending" sheetId="4" r:id="rId1"/>
@@ -1504,11 +1504,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3922,10 +3922,10 @@
   <dimension ref="A1:V104"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C103" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6088,11 +6088,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V100"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B38" sqref="B38"/>
+      <selection pane="bottomRight" activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>